<commit_message>
delete record functionality removed from the app
</commit_message>
<xml_diff>
--- a/vehicle_data.xlsx
+++ b/vehicle_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,6 +635,32 @@
         <v>5000</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>GM0011</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>03/20/2025 06:25:21 PM</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ba kha 1111</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2100</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9100</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>